<commit_message>
made updates to main.py and output_myactivity
</commit_message>
<xml_diff>
--- a/output_myactivity.xlsx
+++ b/output_myactivity.xlsx
@@ -476,7 +476,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>Sunday Dinner</t>
+          <t>Pasta</t>
         </is>
       </c>
     </row>
@@ -516,17 +516,17 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Like to watch movies</t>
+          <t>Watch movies</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
+          <t>Listen to music</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
           <t>Go for walks</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Painting</t>
         </is>
       </c>
     </row>
@@ -566,7 +566,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Little Women</t>
+          <t>The Secret</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">

</xml_diff>